<commit_message>
Atualização das ementas de qualidade.
</commit_message>
<xml_diff>
--- a/ch_01.xlsx
+++ b/ch_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Documents\dev\relatorios\ppc_ciencia_de_dados_unifei\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F28122-2870-4817-B489-35D7C9CF17E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C33C29-6CC1-421F-A45C-8355690D5C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3570" yWindow="8002" windowWidth="21795" windowHeight="12975" xr2:uid="{449215E2-5059-4847-B8DB-C48B4239A68A}"/>
+    <workbookView xWindow="-3472" yWindow="9720" windowWidth="21600" windowHeight="11160" activeTab="2" xr2:uid="{449215E2-5059-4847-B8DB-C48B4239A68A}"/>
   </bookViews>
   <sheets>
     <sheet name="ch_total" sheetId="1" r:id="rId1"/>
@@ -332,7 +332,7 @@
     <t>Industria 4.0: Conceitos e Fundamentos</t>
   </si>
   <si>
-    <t>Engenharia da Qualidade 2</t>
+    <t>Projeto e Análise de Experimentos</t>
   </si>
 </sst>
 </file>
@@ -877,7 +877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E895C6EF-A189-46BF-83CE-105DCC7C97EF}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -926,11 +926,11 @@
         <v>240</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C8" si="0">ROUND(D3,0)</f>
+        <f t="shared" ref="C3:C7" si="0">ROUND(D3,0)</f>
         <v>200</v>
       </c>
       <c r="D3" s="6">
-        <f t="shared" ref="D3:D8" si="1">5/6*B3</f>
+        <f t="shared" ref="D3:D7" si="1">5/6*B3</f>
         <v>200</v>
       </c>
     </row>
@@ -1084,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70238A55-2A6A-4AA7-ADB1-0340B6F3E254}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Atualização da grade curricular dos dois primeiros semestres
</commit_message>
<xml_diff>
--- a/ch_01.xlsx
+++ b/ch_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Documents\dev\relatorios\ppc_ciencia_de_dados_unifei\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C33C29-6CC1-421F-A45C-8355690D5C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E8593F-067F-424B-BD5A-F3C8B9744402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3472" yWindow="9720" windowWidth="21600" windowHeight="11160" activeTab="2" xr2:uid="{449215E2-5059-4847-B8DB-C48B4239A68A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{449215E2-5059-4847-B8DB-C48B4239A68A}"/>
   </bookViews>
   <sheets>
     <sheet name="ch_total" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="esporte" sheetId="5" r:id="rId5"/>
     <sheet name="gestao" sheetId="6" r:id="rId6"/>
     <sheet name="optativas" sheetId="7" r:id="rId7"/>
+    <sheet name="ch_semestre (2)" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="119">
   <si>
     <t>Elemento</t>
   </si>
@@ -329,17 +330,83 @@
     <t>Visualização de Dados</t>
   </si>
   <si>
-    <t>Industria 4.0: Conceitos e Fundamentos</t>
-  </si>
-  <si>
     <t>Projeto e Análise de Experimentos</t>
+  </si>
+  <si>
+    <t>Técnicas de Amostragem</t>
+  </si>
+  <si>
+    <t>Estatístico</t>
+  </si>
+  <si>
+    <t>Rodrigo Lima</t>
+  </si>
+  <si>
+    <t>João</t>
+  </si>
+  <si>
+    <t>Usinagem</t>
+  </si>
+  <si>
+    <t>Matheus</t>
+  </si>
+  <si>
+    <t>contratar</t>
+  </si>
+  <si>
+    <t>Liberação de carga</t>
+  </si>
+  <si>
+    <t>Computação</t>
+  </si>
+  <si>
+    <t>Victor/Moisés</t>
+  </si>
+  <si>
+    <t>Saúde</t>
+  </si>
+  <si>
+    <t>Esporte</t>
+  </si>
+  <si>
+    <t>1ª</t>
+  </si>
+  <si>
+    <t>2ª</t>
+  </si>
+  <si>
+    <t>6ª</t>
+  </si>
+  <si>
+    <t>Economia</t>
+  </si>
+  <si>
+    <t>7ª</t>
+  </si>
+  <si>
+    <t>8ª</t>
+  </si>
+  <si>
+    <t>9ª</t>
+  </si>
+  <si>
+    <t>Engenharia</t>
+  </si>
+  <si>
+    <t>3ª</t>
+  </si>
+  <si>
+    <t>4ª/5ª</t>
+  </si>
+  <si>
+    <t>estudo de perfil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,8 +446,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,8 +466,62 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -478,11 +605,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -540,6 +676,107 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1084,8 +1321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70238A55-2A6A-4AA7-ADB1-0340B6F3E254}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1441,7 +1678,7 @@
         <v>3</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L7" s="11">
         <v>3</v>
@@ -1459,7 +1696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>2</v>
       </c>
@@ -1467,7 +1704,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="D8" s="11">
         <v>2</v>
@@ -1479,7 +1716,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="H8" s="11">
         <v>2</v>
@@ -1812,4 +2049,606 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{483CE0CC-FCC6-471D-8C22-D5EF56686AEB}">
+  <dimension ref="A1:P22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="4.28515625" style="4" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="23">
+        <v>4</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="23">
+        <v>4</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="41">
+        <v>4</v>
+      </c>
+      <c r="G2" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="57">
+        <v>6</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="22">
+        <v>3</v>
+      </c>
+      <c r="K2" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="57">
+        <v>6</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="42">
+        <v>3</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="23">
+        <v>3</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="30">
+        <v>3</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="31">
+        <v>3</v>
+      </c>
+      <c r="I3" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="38">
+        <v>4</v>
+      </c>
+      <c r="K3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" s="42">
+        <v>3</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="N3" s="11">
+        <v>3</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="22">
+        <v>3</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="37">
+        <v>2</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="27">
+        <v>3</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="35">
+        <v>3</v>
+      </c>
+      <c r="I4" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="34">
+        <v>2</v>
+      </c>
+      <c r="K4" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="29">
+        <v>3</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" s="11">
+        <v>3</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="33">
+        <v>3</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="56">
+        <v>3</v>
+      </c>
+      <c r="E5" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="57">
+        <v>2</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="22">
+        <v>3</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="22">
+        <v>3</v>
+      </c>
+      <c r="K5" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="42">
+        <v>3</v>
+      </c>
+      <c r="M5" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="38">
+        <v>3</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="38">
+        <v>3</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="38">
+        <v>3</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="38">
+        <v>3</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="39">
+        <v>3</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="38">
+        <v>3</v>
+      </c>
+      <c r="K6" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="22">
+        <v>3</v>
+      </c>
+      <c r="M6" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="29">
+        <v>3</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="29">
+        <v>3</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="43">
+        <v>3</v>
+      </c>
+      <c r="E7" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="57">
+        <v>2</v>
+      </c>
+      <c r="G7" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="57">
+        <v>3</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="11">
+        <v>3</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="L7" s="22">
+        <v>3</v>
+      </c>
+      <c r="M7" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="N7" s="34">
+        <v>3</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="22">
+        <v>2</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="11">
+        <v>3</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="11">
+        <v>2</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" s="11">
+        <v>3</v>
+      </c>
+      <c r="K8" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="L8" s="34">
+        <v>3</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="P8" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="52">
+        <v>1</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="40">
+        <v>1</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="44"/>
+      <c r="D15" s="45">
+        <v>1</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+    </row>
+    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="55"/>
+      <c r="D16" s="53">
+        <v>2</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="48"/>
+      <c r="D17" s="47">
+        <v>1</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="48"/>
+      <c r="D18" s="47">
+        <v>1</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B16:C16"/>
+  </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Atualização das siglas das disciplinas de primeiro semestre.
</commit_message>
<xml_diff>
--- a/ch_01.xlsx
+++ b/ch_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Documents\dev\relatorios\ppc_ciencia_de_dados_unifei\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E8593F-067F-424B-BD5A-F3C8B9744402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3687EAE-D770-4230-B2DF-2513AC33E258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{449215E2-5059-4847-B8DB-C48B4239A68A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{449215E2-5059-4847-B8DB-C48B4239A68A}"/>
   </bookViews>
   <sheets>
     <sheet name="ch_total" sheetId="1" r:id="rId1"/>
@@ -705,9 +705,6 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -727,9 +724,6 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -738,9 +732,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -749,34 +740,43 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1321,7 +1321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70238A55-2A6A-4AA7-ADB1-0340B6F3E254}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -2055,8 +2055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{483CE0CC-FCC6-471D-8C22-D5EF56686AEB}">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:M9"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2146,13 +2146,13 @@
       <c r="E2" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="41">
+      <c r="F2" s="39">
         <v>4</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="57">
+      <c r="H2" s="49">
         <v>6</v>
       </c>
       <c r="I2" s="22" t="s">
@@ -2161,10 +2161,10 @@
       <c r="J2" s="22">
         <v>3</v>
       </c>
-      <c r="K2" s="58" t="s">
+      <c r="K2" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="57">
+      <c r="L2" s="49">
         <v>6</v>
       </c>
       <c r="M2" s="11" t="s">
@@ -2181,10 +2181,10 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="42">
+      <c r="B3" s="40">
         <v>3</v>
       </c>
       <c r="C3" s="23" t="s">
@@ -2205,16 +2205,16 @@
       <c r="H3" s="31">
         <v>3</v>
       </c>
-      <c r="I3" s="38" t="s">
+      <c r="I3" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="38">
+      <c r="J3" s="37">
         <v>4</v>
       </c>
-      <c r="K3" s="42" t="s">
+      <c r="K3" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="L3" s="42">
+      <c r="L3" s="40">
         <v>3</v>
       </c>
       <c r="M3" s="11" t="s">
@@ -2240,7 +2240,7 @@
       <c r="C4" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="36">
         <v>2</v>
       </c>
       <c r="E4" s="26" t="s">
@@ -2249,16 +2249,16 @@
       <c r="F4" s="27">
         <v>3</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="35">
-        <v>3</v>
-      </c>
-      <c r="I4" s="33" t="s">
+      <c r="H4" s="34">
+        <v>3</v>
+      </c>
+      <c r="I4" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="34">
+      <c r="J4" s="33">
         <v>2</v>
       </c>
       <c r="K4" s="29" t="s">
@@ -2281,22 +2281,22 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="33">
-        <v>3</v>
-      </c>
-      <c r="C5" s="56" t="s">
+      <c r="B5" s="32">
+        <v>3</v>
+      </c>
+      <c r="C5" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="56">
-        <v>3</v>
-      </c>
-      <c r="E5" s="57" t="s">
+      <c r="D5" s="48">
+        <v>3</v>
+      </c>
+      <c r="E5" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="57">
+      <c r="F5" s="49">
         <v>2</v>
       </c>
       <c r="G5" s="22" t="s">
@@ -2311,16 +2311,16 @@
       <c r="J5" s="22">
         <v>3</v>
       </c>
-      <c r="K5" s="42" t="s">
+      <c r="K5" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="42">
-        <v>3</v>
-      </c>
-      <c r="M5" s="38" t="s">
+      <c r="L5" s="40">
+        <v>3</v>
+      </c>
+      <c r="M5" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="38">
+      <c r="N5" s="37">
         <v>3</v>
       </c>
       <c r="O5" s="11" t="s">
@@ -2331,34 +2331,34 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="38">
-        <v>3</v>
-      </c>
-      <c r="C6" s="38" t="s">
+      <c r="B6" s="37">
+        <v>3</v>
+      </c>
+      <c r="C6" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="38">
-        <v>3</v>
-      </c>
-      <c r="E6" s="38" t="s">
+      <c r="D6" s="37">
+        <v>3</v>
+      </c>
+      <c r="E6" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="38">
-        <v>3</v>
-      </c>
-      <c r="G6" s="38" t="s">
+      <c r="F6" s="37">
+        <v>3</v>
+      </c>
+      <c r="G6" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="39">
-        <v>3</v>
-      </c>
-      <c r="I6" s="38" t="s">
+      <c r="H6" s="38">
+        <v>3</v>
+      </c>
+      <c r="I6" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="38">
+      <c r="J6" s="37">
         <v>3</v>
       </c>
       <c r="K6" s="22" t="s">
@@ -2387,22 +2387,22 @@
       <c r="B7" s="29">
         <v>3</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="D7" s="43">
-        <v>3</v>
-      </c>
-      <c r="E7" s="57" t="s">
+      <c r="D7" s="41">
+        <v>3</v>
+      </c>
+      <c r="E7" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="57">
-        <v>2</v>
-      </c>
-      <c r="G7" s="57" t="s">
+      <c r="F7" s="49">
+        <v>2</v>
+      </c>
+      <c r="G7" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="57">
+      <c r="H7" s="49">
         <v>3</v>
       </c>
       <c r="I7" s="11" t="s">
@@ -2417,10 +2417,10 @@
       <c r="L7" s="22">
         <v>3</v>
       </c>
-      <c r="M7" s="34" t="s">
+      <c r="M7" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="34">
+      <c r="N7" s="33">
         <v>3</v>
       </c>
       <c r="O7" s="11" t="s">
@@ -2461,10 +2461,10 @@
       <c r="J8" s="11">
         <v>3</v>
       </c>
-      <c r="K8" s="34" t="s">
+      <c r="K8" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="L8" s="34">
+      <c r="L8" s="33">
         <v>3</v>
       </c>
       <c r="M8" s="11" t="s">
@@ -2481,60 +2481,75 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="52">
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="46">
         <v>1</v>
       </c>
       <c r="E10" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="F10" s="24"/>
+      <c r="F10" s="4">
+        <f>SUM(F2:F8)</f>
+        <v>20</v>
+      </c>
       <c r="G10" s="24"/>
+      <c r="H10" s="4">
+        <f>SUM(H2:H8)</f>
+        <v>23</v>
+      </c>
+      <c r="J10" s="4">
+        <f>SUM(J2:J8)</f>
+        <v>21</v>
+      </c>
+      <c r="L10" s="4">
+        <f>SUM(L2:L8)</f>
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
       <c r="E11" s="24"/>
       <c r="F11" s="24"/>
       <c r="G11" s="24"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
       <c r="E12" s="24"/>
       <c r="F12" s="24"/>
       <c r="G12" s="24"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
       <c r="E13" s="24"/>
       <c r="F13" s="24"/>
       <c r="G13" s="24"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="40">
+      <c r="C14" s="54"/>
+      <c r="D14" s="25">
         <v>1</v>
       </c>
       <c r="E14" s="24" t="s">
@@ -2544,14 +2559,14 @@
       <c r="G14" s="24"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="45">
+      <c r="C15" s="55"/>
+      <c r="D15" s="42">
         <v>1</v>
       </c>
       <c r="E15" s="24" t="s">
@@ -2561,14 +2576,14 @@
       <c r="G15" s="24"/>
     </row>
     <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="C16" s="55"/>
-      <c r="D16" s="53">
+      <c r="C16" s="58"/>
+      <c r="D16" s="47">
         <v>2</v>
       </c>
       <c r="E16" s="24" t="s">
@@ -2578,14 +2593,14 @@
       <c r="G16" s="24"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="47">
+      <c r="C17" s="51"/>
+      <c r="D17" s="44">
         <v>1</v>
       </c>
       <c r="E17" s="24" t="s">
@@ -2597,14 +2612,14 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="48"/>
-      <c r="D18" s="47">
+      <c r="C18" s="51"/>
+      <c r="D18" s="44">
         <v>1</v>
       </c>
       <c r="E18" s="24" t="s">

</xml_diff>

<commit_message>
Atualização das ementas finalizadas.
</commit_message>
<xml_diff>
--- a/ch_01.xlsx
+++ b/ch_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Documents\dev\relatorios\ppc_ciencia_de_dados_unifei\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3687EAE-D770-4230-B2DF-2513AC33E258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B465C339-375F-4E47-AC48-1B6EAB7D695B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{449215E2-5059-4847-B8DB-C48B4239A68A}"/>
+    <workbookView xWindow="-21690" yWindow="18840" windowWidth="21780" windowHeight="18930" activeTab="2" xr2:uid="{449215E2-5059-4847-B8DB-C48B4239A68A}"/>
   </bookViews>
   <sheets>
     <sheet name="ch_total" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="121">
   <si>
     <t>Elemento</t>
   </si>
@@ -400,6 +400,12 @@
   </si>
   <si>
     <t>estudo de perfil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Séries Temporais </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modelos em Painel e Instrumentos </t>
   </si>
 </sst>
 </file>
@@ -453,7 +459,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -520,8 +526,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -614,11 +626,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -647,28 +672,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -695,7 +702,6 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -741,7 +747,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -757,9 +762,6 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -776,6 +778,40 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1141,17 +1177,17 @@
       <c r="A2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="2">
-        <f>(ch_semestre!B2+ch_semestre!B3+ch_semestre!B4+ch_semestre!B5+ch_semestre!B6+ch_semestre!B7+ch_semestre!D2+ch_semestre!D3+ch_semestre!D4+ch_semestre!D5+ch_semestre!D6+ch_semestre!D7+ch_semestre!D8+ch_semestre!F2+ch_semestre!F3+ch_semestre!F4+ch_semestre!F5+ch_semestre!F6+ch_semestre!F7+ch_semestre!F8+ch_semestre!H2+ch_semestre!H3+ch_semestre!H4+ch_semestre!H5+ch_semestre!H6+ch_semestre!H7+ch_semestre!H8+ch_semestre!J2+ch_semestre!J3+ch_semestre!J4+ch_semestre!J5+ch_semestre!J6+ch_semestre!J7+ch_semestre!J8+ch_semestre!L8+ch_semestre!L7+ch_semestre!L4+ch_semestre!L3+ch_semestre!L2+ch_semestre!N3+ch_semestre!N4)*16</f>
-        <v>2032</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="2" t="e">
+        <f>(ch_semestre!B2+ch_semestre!B3+ch_semestre!B4+ch_semestre!B5+ch_semestre!B6+ch_semestre!B7+ch_semestre!D2+ch_semestre!D3+ch_semestre!D4+ch_semestre!D5+ch_semestre!D6+ch_semestre!D7+ch_semestre!D8+ch_semestre!F2+ch_semestre!F3+ch_semestre!F4+ch_semestre!F5+ch_semestre!F6+ch_semestre!F7+ch_semestre!#REF!+ch_semestre!H2+ch_semestre!H3+ch_semestre!H4+ch_semestre!H5+ch_semestre!H6+ch_semestre!H7+ch_semestre!F8+ch_semestre!J2+ch_semestre!J3+ch_semestre!J4+ch_semestre!J5+ch_semestre!J6+ch_semestre!J7+ch_semestre!N3+ch_semestre!L8+ch_semestre!L7+ch_semestre!L4+ch_semestre!L3+ch_semestre!L2+ch_semestre!#REF!+ch_semestre!N4)*16</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C2" s="2" t="e">
         <f>ROUND(D2,0)</f>
-        <v>1693</v>
-      </c>
-      <c r="D2" s="6">
+        <v>#REF!</v>
+      </c>
+      <c r="D2" s="6" t="e">
         <f>5/6*B2</f>
-        <v>1693.3333333333335</v>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1239,17 +1275,17 @@
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="2" t="e">
         <f>SUM(B2:B7)</f>
-        <v>3870</v>
-      </c>
-      <c r="C8" s="2">
+        <v>#REF!</v>
+      </c>
+      <c r="C8" s="2" t="e">
         <f>ROUND(D8,0)</f>
-        <v>3225</v>
-      </c>
-      <c r="D8" s="6">
+        <v>#REF!</v>
+      </c>
+      <c r="D8" s="6" t="e">
         <f>5/6*B8</f>
-        <v>3225</v>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>
@@ -1319,10 +1355,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70238A55-2A6A-4AA7-ADB1-0340B6F3E254}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1397,358 +1433,354 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="50">
         <v>4</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="50">
         <v>4</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="51">
         <v>4</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="50">
         <v>6</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="11">
-        <v>3</v>
-      </c>
-      <c r="K2" s="13" t="s">
+      <c r="J2" s="50">
+        <v>3</v>
+      </c>
+      <c r="K2" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="11">
+      <c r="L2" s="50">
         <v>6</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="N2" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="O2" s="11" t="s">
+      <c r="N2" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="53" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="11">
-        <v>3</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="50">
+        <v>3</v>
+      </c>
+      <c r="C3" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="11">
-        <v>3</v>
-      </c>
-      <c r="E3" s="11" t="s">
+      <c r="D3" s="50">
+        <v>3</v>
+      </c>
+      <c r="E3" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="12">
-        <v>3</v>
-      </c>
-      <c r="G3" s="11" t="s">
+      <c r="F3" s="51">
+        <v>3</v>
+      </c>
+      <c r="G3" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="15">
-        <v>3</v>
-      </c>
-      <c r="I3" s="11" t="s">
+      <c r="H3" s="54">
+        <v>3</v>
+      </c>
+      <c r="I3" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="50">
         <v>4</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="L3" s="11">
-        <v>3</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="N3" s="11">
-        <v>3</v>
-      </c>
-      <c r="O3" s="16" t="s">
+      <c r="L3" s="50">
+        <v>3</v>
+      </c>
+      <c r="M3" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" s="50">
+        <v>3</v>
+      </c>
+      <c r="O3" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="P3" s="53" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="11">
-        <v>3</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="50">
+        <v>3</v>
+      </c>
+      <c r="C4" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="12">
-        <v>2</v>
-      </c>
-      <c r="E4" s="16" t="s">
+      <c r="D4" s="51">
+        <v>2</v>
+      </c>
+      <c r="E4" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="17">
-        <v>3</v>
-      </c>
-      <c r="G4" s="16" t="s">
+      <c r="F4" s="56">
+        <v>3</v>
+      </c>
+      <c r="G4" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="18">
-        <v>3</v>
-      </c>
-      <c r="I4" s="16" t="s">
+      <c r="H4" s="57">
+        <v>3</v>
+      </c>
+      <c r="I4" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="11">
-        <v>2</v>
-      </c>
-      <c r="K4" s="11" t="s">
+      <c r="J4" s="50">
+        <v>2</v>
+      </c>
+      <c r="K4" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="11">
-        <v>3</v>
-      </c>
-      <c r="M4" s="11" t="s">
+      <c r="L4" s="50">
+        <v>3</v>
+      </c>
+      <c r="M4" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="N4" s="11">
-        <v>3</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="P4" s="11" t="s">
+      <c r="N4" s="50">
+        <v>3</v>
+      </c>
+      <c r="O4" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="50" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="16">
-        <v>3</v>
-      </c>
-      <c r="C5" s="16" t="s">
+      <c r="B5" s="55">
+        <v>3</v>
+      </c>
+      <c r="C5" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="16">
-        <v>3</v>
-      </c>
-      <c r="E5" s="11" t="s">
+      <c r="D5" s="55">
+        <v>3</v>
+      </c>
+      <c r="E5" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="11">
-        <v>2</v>
-      </c>
-      <c r="G5" s="11" t="s">
+      <c r="F5" s="50">
+        <v>2</v>
+      </c>
+      <c r="G5" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="11">
-        <v>3</v>
-      </c>
-      <c r="I5" s="11" t="s">
+      <c r="H5" s="50">
+        <v>3</v>
+      </c>
+      <c r="I5" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="11">
-        <v>3</v>
-      </c>
-      <c r="K5" s="11" t="s">
+      <c r="J5" s="50">
+        <v>3</v>
+      </c>
+      <c r="K5" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="11">
-        <v>3</v>
-      </c>
-      <c r="M5" s="11" t="s">
+      <c r="L5" s="50">
+        <v>3</v>
+      </c>
+      <c r="M5" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="11">
-        <v>3</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="P5" s="11" t="s">
+      <c r="N5" s="50">
+        <v>3</v>
+      </c>
+      <c r="O5" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" s="50" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="11">
-        <v>3</v>
-      </c>
-      <c r="C6" s="11" t="s">
+      <c r="B6" s="50">
+        <v>3</v>
+      </c>
+      <c r="C6" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="11">
-        <v>3</v>
-      </c>
-      <c r="E6" s="11" t="s">
+      <c r="D6" s="50">
+        <v>3</v>
+      </c>
+      <c r="E6" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="11">
-        <v>3</v>
-      </c>
-      <c r="G6" s="11" t="s">
+      <c r="F6" s="50">
+        <v>3</v>
+      </c>
+      <c r="G6" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="15">
-        <v>3</v>
-      </c>
-      <c r="I6" s="11" t="s">
+      <c r="H6" s="54">
+        <v>3</v>
+      </c>
+      <c r="I6" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="11">
-        <v>3</v>
-      </c>
-      <c r="K6" s="11" t="s">
+      <c r="J6" s="50">
+        <v>3</v>
+      </c>
+      <c r="K6" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="11">
-        <v>3</v>
-      </c>
-      <c r="M6" s="11" t="s">
+      <c r="L6" s="50">
+        <v>3</v>
+      </c>
+      <c r="M6" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="11">
-        <v>3</v>
-      </c>
-      <c r="O6" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="P6" s="11" t="s">
+      <c r="N6" s="50">
+        <v>3</v>
+      </c>
+      <c r="O6" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" s="50" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="11">
-        <v>3</v>
-      </c>
-      <c r="C7" s="11" t="s">
+      <c r="B7" s="50">
+        <v>3</v>
+      </c>
+      <c r="C7" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="D7" s="16">
-        <v>3</v>
-      </c>
-      <c r="E7" s="11" t="s">
+      <c r="D7" s="55">
+        <v>3</v>
+      </c>
+      <c r="E7" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="11">
-        <v>2</v>
-      </c>
-      <c r="G7" s="11" t="s">
+      <c r="F7" s="50">
+        <v>2</v>
+      </c>
+      <c r="G7" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="11">
-        <v>3</v>
-      </c>
-      <c r="I7" s="11" t="s">
+      <c r="H7" s="50">
+        <v>3</v>
+      </c>
+      <c r="I7" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="11">
-        <v>3</v>
-      </c>
-      <c r="K7" s="11" t="s">
+      <c r="J7" s="50">
+        <v>3</v>
+      </c>
+      <c r="K7" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="L7" s="11">
-        <v>3</v>
-      </c>
-      <c r="M7" s="11" t="s">
+      <c r="L7" s="50">
+        <v>3</v>
+      </c>
+      <c r="M7" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="11">
-        <v>3</v>
-      </c>
-      <c r="O7" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="P7" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="11" t="s">
+      <c r="N7" s="50">
+        <v>3</v>
+      </c>
+      <c r="O7" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="50" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="11">
-        <v>2</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="11">
-        <v>3</v>
-      </c>
-      <c r="G8" s="11" t="s">
+      <c r="D8" s="50">
+        <v>2</v>
+      </c>
+      <c r="E8" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="11">
-        <v>2</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="J8" s="11">
-        <v>3</v>
-      </c>
-      <c r="K8" s="11" t="s">
+      <c r="F8" s="50">
+        <v>2</v>
+      </c>
+      <c r="G8" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="H8" s="58">
+        <v>3</v>
+      </c>
+      <c r="I8" s="59" t="s">
+        <v>120</v>
+      </c>
+      <c r="J8" s="58">
+        <v>3</v>
+      </c>
+      <c r="K8" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="L8" s="11">
-        <v>3</v>
-      </c>
-      <c r="M8" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="N8" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="O8" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="P8" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="E10" s="19"/>
-      <c r="I10" s="19"/>
+      <c r="L8" s="50">
+        <v>3</v>
+      </c>
+      <c r="M8" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="O8" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="P8" s="50" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1782,7 +1814,7 @@
       <c r="A2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="14">
         <v>48</v>
       </c>
     </row>
@@ -1790,7 +1822,7 @@
       <c r="A3" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="14">
         <v>48</v>
       </c>
     </row>
@@ -1798,7 +1830,7 @@
       <c r="A4" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="14">
         <v>48</v>
       </c>
     </row>
@@ -1806,7 +1838,7 @@
       <c r="A5" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="14">
         <v>48</v>
       </c>
     </row>
@@ -1842,7 +1874,7 @@
       <c r="A2" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="14">
         <v>48</v>
       </c>
     </row>
@@ -1850,7 +1882,7 @@
       <c r="A3" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="14">
         <v>48</v>
       </c>
     </row>
@@ -1858,7 +1890,7 @@
       <c r="A4" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="14">
         <v>48</v>
       </c>
     </row>
@@ -1866,7 +1898,7 @@
       <c r="A5" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="14">
         <v>48</v>
       </c>
     </row>
@@ -1874,7 +1906,7 @@
       <c r="A6" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="14">
         <v>48</v>
       </c>
     </row>
@@ -1882,7 +1914,7 @@
       <c r="A7" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="14">
         <v>48</v>
       </c>
     </row>
@@ -1918,7 +1950,7 @@
       <c r="A2" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="14">
         <v>48</v>
       </c>
     </row>
@@ -1926,7 +1958,7 @@
       <c r="A3" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="14">
         <v>48</v>
       </c>
     </row>
@@ -1934,7 +1966,7 @@
       <c r="A4" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="14">
         <v>48</v>
       </c>
     </row>
@@ -1942,7 +1974,7 @@
       <c r="A5" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="14">
         <v>48</v>
       </c>
     </row>
@@ -1950,7 +1982,7 @@
       <c r="A6" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="14">
         <v>48</v>
       </c>
     </row>
@@ -1958,7 +1990,7 @@
       <c r="A7" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="14">
         <v>48</v>
       </c>
     </row>
@@ -1994,7 +2026,7 @@
       <c r="A2" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="14">
         <v>48</v>
       </c>
     </row>
@@ -2002,7 +2034,7 @@
       <c r="A3" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="14">
         <v>48</v>
       </c>
     </row>
@@ -2010,7 +2042,7 @@
       <c r="A4" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="14">
         <v>48</v>
       </c>
     </row>
@@ -2018,7 +2050,7 @@
       <c r="A5" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="14">
         <v>48</v>
       </c>
     </row>
@@ -2026,7 +2058,7 @@
       <c r="A6" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="14">
         <v>48</v>
       </c>
     </row>
@@ -2034,7 +2066,7 @@
       <c r="A7" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="14">
         <v>48</v>
       </c>
     </row>
@@ -2042,7 +2074,7 @@
       <c r="A8" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2056,7 +2088,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2131,90 +2163,90 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="23">
+      <c r="B2" s="17">
         <v>4</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="17">
         <v>4</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="39">
+      <c r="F2" s="32">
         <v>4</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="49">
+      <c r="H2" s="41">
         <v>6</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="22">
-        <v>3</v>
-      </c>
-      <c r="K2" s="50" t="s">
+      <c r="J2" s="16">
+        <v>3</v>
+      </c>
+      <c r="K2" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="49">
+      <c r="L2" s="41">
         <v>6</v>
       </c>
       <c r="M2" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="O2" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="12" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="40">
-        <v>3</v>
-      </c>
-      <c r="C3" s="23" t="s">
+      <c r="B3" s="33">
+        <v>3</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="23">
-        <v>3</v>
-      </c>
-      <c r="E3" s="29" t="s">
+      <c r="D3" s="17">
+        <v>3</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="30">
-        <v>3</v>
-      </c>
-      <c r="G3" s="29" t="s">
+      <c r="F3" s="23">
+        <v>3</v>
+      </c>
+      <c r="G3" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="31">
-        <v>3</v>
-      </c>
-      <c r="I3" s="37" t="s">
+      <c r="H3" s="24">
+        <v>3</v>
+      </c>
+      <c r="I3" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="37">
+      <c r="J3" s="30">
         <v>4</v>
       </c>
-      <c r="K3" s="40" t="s">
+      <c r="K3" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="L3" s="40">
+      <c r="L3" s="33">
         <v>3</v>
       </c>
       <c r="M3" s="11" t="s">
@@ -2223,48 +2255,48 @@
       <c r="N3" s="11">
         <v>3</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="O3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="P3" s="12" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="22">
-        <v>3</v>
-      </c>
-      <c r="C4" s="22" t="s">
+      <c r="B4" s="16">
+        <v>3</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="36">
-        <v>2</v>
-      </c>
-      <c r="E4" s="26" t="s">
+      <c r="D4" s="29">
+        <v>2</v>
+      </c>
+      <c r="E4" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="27">
-        <v>3</v>
-      </c>
-      <c r="G4" s="32" t="s">
+      <c r="F4" s="21">
+        <v>3</v>
+      </c>
+      <c r="G4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="34">
-        <v>3</v>
-      </c>
-      <c r="I4" s="32" t="s">
+      <c r="H4" s="27">
+        <v>3</v>
+      </c>
+      <c r="I4" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="33">
-        <v>2</v>
-      </c>
-      <c r="K4" s="29" t="s">
+      <c r="J4" s="26">
+        <v>2</v>
+      </c>
+      <c r="K4" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="29">
+      <c r="L4" s="22">
         <v>3</v>
       </c>
       <c r="M4" s="11" t="s">
@@ -2281,46 +2313,46 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="32">
-        <v>3</v>
-      </c>
-      <c r="C5" s="48" t="s">
+      <c r="B5" s="25">
+        <v>3</v>
+      </c>
+      <c r="C5" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="48">
-        <v>3</v>
-      </c>
-      <c r="E5" s="49" t="s">
+      <c r="D5" s="40">
+        <v>3</v>
+      </c>
+      <c r="E5" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="49">
-        <v>2</v>
-      </c>
-      <c r="G5" s="22" t="s">
+      <c r="F5" s="41">
+        <v>2</v>
+      </c>
+      <c r="G5" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="22">
-        <v>3</v>
-      </c>
-      <c r="I5" s="22" t="s">
+      <c r="H5" s="16">
+        <v>3</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="22">
-        <v>3</v>
-      </c>
-      <c r="K5" s="40" t="s">
+      <c r="J5" s="16">
+        <v>3</v>
+      </c>
+      <c r="K5" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="40">
-        <v>3</v>
-      </c>
-      <c r="M5" s="37" t="s">
+      <c r="L5" s="33">
+        <v>3</v>
+      </c>
+      <c r="M5" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="37">
+      <c r="N5" s="30">
         <v>3</v>
       </c>
       <c r="O5" s="11" t="s">
@@ -2331,46 +2363,46 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="37">
-        <v>3</v>
-      </c>
-      <c r="C6" s="37" t="s">
+      <c r="B6" s="30">
+        <v>3</v>
+      </c>
+      <c r="C6" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="37">
-        <v>3</v>
-      </c>
-      <c r="E6" s="37" t="s">
+      <c r="D6" s="30">
+        <v>3</v>
+      </c>
+      <c r="E6" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="37">
-        <v>3</v>
-      </c>
-      <c r="G6" s="37" t="s">
+      <c r="F6" s="30">
+        <v>3</v>
+      </c>
+      <c r="G6" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="38">
-        <v>3</v>
-      </c>
-      <c r="I6" s="37" t="s">
+      <c r="H6" s="31">
+        <v>3</v>
+      </c>
+      <c r="I6" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="37">
-        <v>3</v>
-      </c>
-      <c r="K6" s="22" t="s">
+      <c r="J6" s="30">
+        <v>3</v>
+      </c>
+      <c r="K6" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="22">
-        <v>3</v>
-      </c>
-      <c r="M6" s="29" t="s">
+      <c r="L6" s="16">
+        <v>3</v>
+      </c>
+      <c r="M6" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="29">
+      <c r="N6" s="22">
         <v>3</v>
       </c>
       <c r="O6" s="11" t="s">
@@ -2381,28 +2413,28 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="29">
-        <v>3</v>
-      </c>
-      <c r="C7" s="40" t="s">
+      <c r="B7" s="22">
+        <v>3</v>
+      </c>
+      <c r="C7" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="D7" s="41">
-        <v>3</v>
-      </c>
-      <c r="E7" s="49" t="s">
+      <c r="D7" s="34">
+        <v>3</v>
+      </c>
+      <c r="E7" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="49">
-        <v>2</v>
-      </c>
-      <c r="G7" s="49" t="s">
+      <c r="F7" s="41">
+        <v>2</v>
+      </c>
+      <c r="G7" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="49">
+      <c r="H7" s="41">
         <v>3</v>
       </c>
       <c r="I7" s="11" t="s">
@@ -2411,16 +2443,16 @@
       <c r="J7" s="11">
         <v>3</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="K7" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="L7" s="22">
-        <v>3</v>
-      </c>
-      <c r="M7" s="33" t="s">
+      <c r="L7" s="16">
+        <v>3</v>
+      </c>
+      <c r="M7" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="33">
+      <c r="N7" s="26">
         <v>3</v>
       </c>
       <c r="O7" s="11" t="s">
@@ -2437,10 +2469,10 @@
       <c r="B8" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="16">
         <v>2</v>
       </c>
       <c r="E8" s="11" t="s">
@@ -2461,10 +2493,10 @@
       <c r="J8" s="11">
         <v>3</v>
       </c>
-      <c r="K8" s="33" t="s">
+      <c r="K8" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="L8" s="33">
+      <c r="L8" s="26">
         <v>3</v>
       </c>
       <c r="M8" s="11" t="s">
@@ -2481,22 +2513,22 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="46">
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="38">
         <v>1</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="18" t="s">
         <v>108</v>
       </c>
       <c r="F10" s="4">
         <f>SUM(F2:F8)</f>
         <v>20</v>
       </c>
-      <c r="G10" s="24"/>
+      <c r="G10" s="18"/>
       <c r="H10" s="4">
         <f>SUM(H2:H8)</f>
         <v>23</v>
@@ -2511,122 +2543,122 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="53"/>
-      <c r="C12" s="53"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="B13" s="56"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="25">
+      <c r="C14" s="45"/>
+      <c r="D14" s="19">
         <v>1</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="C15" s="55"/>
-      <c r="D15" s="42">
+      <c r="C15" s="46"/>
+      <c r="D15" s="35">
         <v>1</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="C16" s="58"/>
-      <c r="D16" s="47">
-        <v>2</v>
-      </c>
-      <c r="E16" s="24" t="s">
+      <c r="C16" s="49"/>
+      <c r="D16" s="39">
+        <v>2</v>
+      </c>
+      <c r="E16" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="44">
+      <c r="C17" s="43"/>
+      <c r="D17" s="37">
         <v>1</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24" t="s">
+      <c r="F17" s="18"/>
+      <c r="G17" s="18" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="51"/>
-      <c r="D18" s="44">
+      <c r="C18" s="43"/>
+      <c r="D18" s="37">
         <v>1</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24" t="s">
+      <c r="F18" s="18"/>
+      <c r="G18" s="18" t="s">
         <v>118</v>
       </c>
     </row>

</xml_diff>